<commit_message>
Update Import Test Case
</commit_message>
<xml_diff>
--- a/front-end/public/template/Example.xlsx
+++ b/front-end/public/template/Example.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TestControl\TestManagementTools\front-end\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8711A3AF-5318-415D-94D7-B9484C6848F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{EA359E8E-22FD-4217-8B3F-BF2531ED4E19}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>Definition</t>
   </si>
@@ -58,37 +57,51 @@
     <t>Description</t>
   </si>
   <si>
-    <t>This is a sample</t>
-  </si>
-  <si>
     <t>Pre-condition</t>
   </si>
   <si>
     <t>Post-condition</t>
   </si>
   <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>Importance</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
     <t>Step</t>
   </si>
   <si>
+    <t>manual</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>This is a sample Test case</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Manual</t>
+  </si>
+  <si>
+    <t>1. Go to Google
+2. Display the object</t>
+  </si>
+  <si>
+    <t>1. Display google websites
+2. Display search result</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
     <t>medium</t>
-  </si>
-  <si>
-    <t>manual</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -106,12 +119,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -154,9 +173,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -164,10 +182,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,71 +505,76 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E54DFA-887E-4B53-9DA5-3FD63E3D081D}">
-  <dimension ref="A1:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="38" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="B2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="E2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -554,10 +583,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16BAEF67-0E6F-48D0-84F2-F499BC88CABE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -569,59 +598,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>12</v>
+      <c r="D1" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>15</v>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>15</v>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Upload Test Case + Template
</commit_message>
<xml_diff>
--- a/front-end/public/template/Example.xlsx
+++ b/front-end/public/template/Example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ldhan\TestManagementTools\front-end\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D046594-FB7B-443E-87DB-AC80F7CDE75A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D339D6CE-74FE-4194-A8A0-1D8338D8EAA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
   <si>
     <t>Definition</t>
   </si>
@@ -87,8 +87,10 @@
     <t>medium</t>
   </si>
   <si>
-    <t>1. manual
-2. auto</t>
+    <t>Sample B</t>
+  </si>
+  <si>
+    <t>As Expected</t>
   </si>
 </sst>
 </file>
@@ -166,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -184,6 +186,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -499,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,8 +570,34 @@
       <c r="G2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>19</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>